<commit_message>
commit in to new branch
</commit_message>
<xml_diff>
--- a/htdocs/2.xlsx
+++ b/htdocs/2.xlsx
@@ -11,6 +11,14 @@
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Hello new branch!</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -350,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,6 +371,11 @@
         <v>2222</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
commit in to branch master
</commit_message>
<xml_diff>
--- a/htdocs/2.xlsx
+++ b/htdocs/2.xlsx
@@ -11,6 +11,14 @@
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>branch master</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -350,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,6 +371,11 @@
         <v>2222</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>